<commit_message>
Aggiornamento revisione su serigrafia scheda (0.3 invece di 1.0). La revisione della scheda sarà la stessa del file .pcbnew
</commit_message>
<xml_diff>
--- a/trunk/KiCAD_ExpansionBoard/TM4C123G_CommExpBoard_BOM.xlsx
+++ b/trunk/KiCAD_ExpansionBoard/TM4C123G_CommExpBoard_BOM.xlsx
@@ -1116,19 +1116,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:J42" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:J42" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:J42"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Valore" dataDxfId="11"/>
-    <tableColumn id="2" name="n°" dataDxfId="10"/>
-    <tableColumn id="3" name="Reference" dataDxfId="9"/>
-    <tableColumn id="4" name="Supplier 1" dataDxfId="8"/>
-    <tableColumn id="5" name="Supplier 1 P/N" dataDxfId="7"/>
-    <tableColumn id="6" name="Manufacturer" dataDxfId="6"/>
-    <tableColumn id="7" name="Manufacturer P/N" dataDxfId="5"/>
-    <tableColumn id="8" name="Description" dataDxfId="4"/>
-    <tableColumn id="9" name="Supplier 2" dataDxfId="3"/>
-    <tableColumn id="10" name="Supplier 2 P/N" dataDxfId="2"/>
+    <tableColumn id="1" name="Valore" dataDxfId="9"/>
+    <tableColumn id="2" name="n°" dataDxfId="8"/>
+    <tableColumn id="3" name="Reference" dataDxfId="7"/>
+    <tableColumn id="4" name="Supplier 1" dataDxfId="6"/>
+    <tableColumn id="5" name="Supplier 1 P/N" dataDxfId="5"/>
+    <tableColumn id="6" name="Manufacturer" dataDxfId="4"/>
+    <tableColumn id="7" name="Manufacturer P/N" dataDxfId="3"/>
+    <tableColumn id="8" name="Description" dataDxfId="2"/>
+    <tableColumn id="9" name="Supplier 2" dataDxfId="1"/>
+    <tableColumn id="10" name="Supplier 2 P/N" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1400,7 +1400,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:J42"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>